<commit_message>
Add data dictionaries to Excel spreadsheets
Each exercise dataset now how a data_dictionary tab.
Also, gender column has been removed from starwars.xlsx.
Leftover temporary file has been removed.
</commit_message>
<xml_diff>
--- a/Excel/data/metro_budget.xlsx
+++ b/Excel/data/metro_budget.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26019"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary van Valkenburg\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAD70D2-3286-47C7-9C4C-6DF3580ADD90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{BAAD70D2-3286-47C7-9C4C-6DF3580ADD90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADAF992F-2F25-409B-818D-4B9B36D48F80}"/>
   <bookViews>
-    <workbookView xWindow="135" yWindow="90" windowWidth="21877" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="135" yWindow="90" windowWidth="21877" windowHeight="13080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
+    <sheet name="data_dictionary" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -23,6 +24,9 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="71">
   <si>
     <t>Department</t>
   </si>
@@ -213,13 +217,43 @@
   </si>
   <si>
     <t>Trustee</t>
+  </si>
+  <si>
+    <t>Metro Nashville government department name</t>
+  </si>
+  <si>
+    <t>Department budget for fiscal year 2017</t>
+  </si>
+  <si>
+    <t>Actual spending for fiscal year 2017</t>
+  </si>
+  <si>
+    <t>Actual spending amount - budget amount for fiscal year 2017</t>
+  </si>
+  <si>
+    <t>Department budget for fiscal year 2018</t>
+  </si>
+  <si>
+    <t>Actual spending for fiscal year 2018</t>
+  </si>
+  <si>
+    <t>Actual spending amount - budget amount for fiscal year 2018</t>
+  </si>
+  <si>
+    <t>Department budget for fiscal year 2019</t>
+  </si>
+  <si>
+    <t>Actual spending for fiscal year 2019</t>
+  </si>
+  <si>
+    <t>Actual spending amount - budget amount for fiscal year 2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -352,6 +386,18 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -702,9 +748,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -764,7 +812,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1052,7 +1100,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1062,24 +1110,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="28.9296875" customWidth="1"/>
-    <col min="2" max="2" width="16.1328125" customWidth="1"/>
-    <col min="3" max="3" width="16.265625" customWidth="1"/>
-    <col min="4" max="4" width="12.53125" customWidth="1"/>
-    <col min="5" max="5" width="15.59765625" customWidth="1"/>
-    <col min="6" max="6" width="12.53125" customWidth="1"/>
-    <col min="7" max="8" width="15.86328125" customWidth="1"/>
-    <col min="9" max="9" width="15.46484375" customWidth="1"/>
-    <col min="10" max="10" width="17.86328125" customWidth="1"/>
+    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="8" width="15.85546875" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1111,7 +1159,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1143,7 +1191,7 @@
         <v>-21269107.77</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1175,7 +1223,7 @@
         <v>-436.96000000001999</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1207,7 +1255,7 @@
         <v>-97416.950000001103</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1239,7 +1287,7 @@
         <v>-262277.08999999898</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1271,7 +1319,7 @@
         <v>-85.710000000079106</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1303,7 +1351,7 @@
         <v>-398759.91999999899</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1335,7 +1383,7 @@
         <v>-241564.68</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1367,7 +1415,7 @@
         <v>-796900.47000000405</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1399,7 +1447,7 @@
         <v>-9181.0800000000108</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1431,7 +1479,7 @@
         <v>-311228.08999999898</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1463,7 +1511,7 @@
         <v>-306086.86</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1495,7 +1543,7 @@
         <v>-150323.329999999</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1527,7 +1575,7 @@
         <v>-21210.119999999901</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1559,7 +1607,7 @@
         <v>-4502589.1500000302</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1591,7 +1639,7 @@
         <v>-106.999999999068</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1623,7 +1671,7 @@
         <v>-965742.96</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1655,7 +1703,7 @@
         <v>-374962.91</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1687,7 +1735,7 @@
         <v>-576344.08999999403</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1719,7 +1767,7 @@
         <v>-116.46000003814601</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1751,7 +1799,7 @@
         <v>-888926.91000000294</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -1783,7 +1831,7 @@
         <v>-745.22999999672095</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -1815,7 +1863,7 @@
         <v>-601242.55999998702</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -1847,7 +1895,7 @@
         <v>-72.879999999888199</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -1879,7 +1927,7 @@
         <v>-1724.8999999999601</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -1911,7 +1959,7 @@
         <v>-313464.78999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -1943,7 +1991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1975,7 +2023,7 @@
         <v>-132614.93999999901</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -2007,7 +2055,7 @@
         <v>-35.329999999143098</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -2039,7 +2087,7 @@
         <v>-35290.389999991203</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -2071,7 +2119,7 @@
         <v>-69308.659999999596</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -2103,7 +2151,7 @@
         <v>-169827.98</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -2135,7 +2183,7 @@
         <v>-5456610.5900001498</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -2167,7 +2215,7 @@
         <v>-115798.49</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -2199,7 +2247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:10">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -2231,7 +2279,7 @@
         <v>-101084.71</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -2263,7 +2311,7 @@
         <v>-188181.66</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:10">
       <c r="A38" t="s">
         <v>46</v>
       </c>
@@ -2295,7 +2343,7 @@
         <v>-136.73999999987399</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:10">
       <c r="A39" t="s">
         <v>47</v>
       </c>
@@ -2327,7 +2375,7 @@
         <v>-79036.130000000296</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:10">
       <c r="A40" t="s">
         <v>48</v>
       </c>
@@ -2359,7 +2407,7 @@
         <v>-610436.29000002099</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:10">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -2391,7 +2439,7 @@
         <v>-82077.349999997707</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:10">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -2423,7 +2471,7 @@
         <v>-36.250000059604602</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:10">
       <c r="A43" t="s">
         <v>51</v>
       </c>
@@ -2455,7 +2503,7 @@
         <v>-346517.43</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:10">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -2487,7 +2535,7 @@
         <v>-58.749999988824101</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:10">
       <c r="A45" t="s">
         <v>53</v>
       </c>
@@ -2519,7 +2567,7 @@
         <v>-640550.34000001801</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:10">
       <c r="A46" t="s">
         <v>54</v>
       </c>
@@ -2551,7 +2599,7 @@
         <v>-12346.84</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:10">
       <c r="A47" t="s">
         <v>55</v>
       </c>
@@ -2583,7 +2631,7 @@
         <v>-21970.8200000822</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:10">
       <c r="A48" t="s">
         <v>56</v>
       </c>
@@ -2615,7 +2663,7 @@
         <v>-407449.76000000199</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:10">
       <c r="A49" t="s">
         <v>57</v>
       </c>
@@ -2647,7 +2695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:10">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -2679,7 +2727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:10">
       <c r="A51" t="s">
         <v>59</v>
       </c>
@@ -2711,7 +2759,7 @@
         <v>-98056.689999999406</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:10">
       <c r="A52" t="s">
         <v>60</v>
       </c>
@@ -2743,7 +2791,7 @@
         <v>-264764.74</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:10">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
@@ -2757,34 +2805,133 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:10">
       <c r="A56" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:10">
       <c r="A57" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:10">
       <c r="A58" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:10">
       <c r="A59" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:10">
       <c r="A60" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:10">
       <c r="A61" t="s">
         <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB99AC6-F6B8-4A26-96BE-D02EE21B4B6C}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>